<commit_message>
Fix bug xong doanh số
</commit_message>
<xml_diff>
--- a/DongAERP/Content/Report/ReportDetailtByPartnerLH.xlsx
+++ b/DongAERP/Content/Report/ReportDetailtByPartnerLH.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DongAERP\DongAERP\Content\Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5410AB1-3BD4-4FD2-A522-932C3872642B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DB4297C-CDBB-40E1-87F1-4DB78D151683}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FDADBC8A-6B6C-45FD-98E5-87326587A42E}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Từ:</t>
   </si>
@@ -63,6 +63,9 @@
   </si>
   <si>
     <t>Doanh số CK</t>
+  </si>
+  <si>
+    <t>USD</t>
   </si>
 </sst>
 </file>
@@ -479,7 +482,7 @@
   <dimension ref="A1:T25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -552,8 +555,11 @@
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="G6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>2</v>
+      </c>
+      <c r="G6" t="s">
+        <v>10</v>
       </c>
       <c r="M6" s="5"/>
       <c r="N6" s="5"/>

</xml_diff>